<commit_message>
Added validation + training loss plot
</commit_message>
<xml_diff>
--- a/predictions/classical_pca_predictions.xlsx
+++ b/predictions/classical_pca_predictions.xlsx
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7725713849067688</v>
+        <v>0.5876173973083496</v>
       </c>
     </row>
     <row r="3">
@@ -485,10 +485,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3531219363212585</v>
+        <v>0.5127014517784119</v>
       </c>
     </row>
     <row r="4">
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8826252222061157</v>
+        <v>0.8669266700744629</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6114453077316284</v>
+        <v>0.8246411681175232</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.08140008896589279</v>
+        <v>0.06286820024251938</v>
       </c>
     </row>
     <row r="7">
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9020189642906189</v>
+        <v>0.8776209354400635</v>
       </c>
     </row>
     <row r="8">
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7517498731613159</v>
+        <v>0.7707201838493347</v>
       </c>
     </row>
     <row r="9">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3957430124282837</v>
+        <v>0.3048694133758545</v>
       </c>
     </row>
     <row r="10">
@@ -611,10 +611,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.522361159324646</v>
+        <v>0.495371550321579</v>
       </c>
     </row>
     <row r="11">
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2734628319740295</v>
+        <v>0.2303283959627151</v>
       </c>
     </row>
     <row r="12">
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.03980230167508125</v>
+        <v>0.1857190877199173</v>
       </c>
     </row>
     <row r="13">
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9540446996688843</v>
+        <v>0.8674956560134888</v>
       </c>
     </row>
     <row r="14">
@@ -686,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8663253784179688</v>
+        <v>0.8751955032348633</v>
       </c>
     </row>
     <row r="15">
@@ -701,10 +701,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.676479697227478</v>
+        <v>0.4216914474964142</v>
       </c>
     </row>
     <row r="16">
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1854447871446609</v>
+        <v>0.2624797523021698</v>
       </c>
     </row>
     <row r="17">
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.944468080997467</v>
+        <v>0.7577654123306274</v>
       </c>
     </row>
     <row r="18">
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8620361089706421</v>
+        <v>0.6054984331130981</v>
       </c>
     </row>
     <row r="19">
@@ -773,10 +773,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6861340999603271</v>
+        <v>0.4093546569347382</v>
       </c>
     </row>
     <row r="20">
@@ -791,10 +791,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6316045522689819</v>
+        <v>0.3960031867027283</v>
       </c>
     </row>
     <row r="21">
@@ -812,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1829105913639069</v>
+        <v>0.1320594996213913</v>
       </c>
     </row>
     <row r="22">
@@ -830,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6996517181396484</v>
+        <v>0.6615296602249146</v>
       </c>
     </row>
     <row r="23">
@@ -848,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7568562626838684</v>
+        <v>0.7411167621612549</v>
       </c>
     </row>
     <row r="24">
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4214471876621246</v>
+        <v>0.4433744549751282</v>
       </c>
     </row>
     <row r="25">
@@ -884,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>0.6805301308631897</v>
+        <v>0.7918363809585571</v>
       </c>
     </row>
     <row r="26">
@@ -902,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>0.802493691444397</v>
+        <v>0.9470779895782471</v>
       </c>
     </row>
     <row r="27">
@@ -920,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2447099089622498</v>
+        <v>0.04427319392561913</v>
       </c>
     </row>
     <row r="28">
@@ -938,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>0.6637791395187378</v>
+        <v>0.8608905076980591</v>
       </c>
     </row>
     <row r="29">
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2935153245925903</v>
+        <v>0.3152673542499542</v>
       </c>
     </row>
     <row r="30">
@@ -974,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0.752056360244751</v>
+        <v>0.7652621269226074</v>
       </c>
     </row>
     <row r="31">
@@ -992,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6251720190048218</v>
+        <v>0.5419816970825195</v>
       </c>
     </row>
     <row r="32">
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>0.6551996469497681</v>
+        <v>0.7014244794845581</v>
       </c>
     </row>
     <row r="33">
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>0.8023707866668701</v>
+        <v>0.722465991973877</v>
       </c>
     </row>
     <row r="34">
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9209647178649902</v>
+        <v>0.907707154750824</v>
       </c>
     </row>
     <row r="35">
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6942132711410522</v>
+        <v>0.6762729287147522</v>
       </c>
     </row>
     <row r="36">
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1380627602338791</v>
+        <v>0.1494694650173187</v>
       </c>
     </row>
     <row r="37">
@@ -1097,10 +1097,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0.6416412591934204</v>
+        <v>0.453951358795166</v>
       </c>
     </row>
     <row r="38">
@@ -1118,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8162031173706055</v>
+        <v>0.8986181616783142</v>
       </c>
     </row>
     <row r="39">
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>0.9467264413833618</v>
+        <v>0.9582871198654175</v>
       </c>
     </row>
     <row r="40">
@@ -1154,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>0.9391160607337952</v>
+        <v>0.8870537877082825</v>
       </c>
     </row>
     <row r="41">
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9826407432556152</v>
+        <v>0.9650564789772034</v>
       </c>
     </row>
     <row r="42">
@@ -1190,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>0.6175154447555542</v>
+        <v>0.5881452560424805</v>
       </c>
     </row>
     <row r="43">
@@ -1208,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>0.7093241810798645</v>
+        <v>0.7852417826652527</v>
       </c>
     </row>
     <row r="44">
@@ -1226,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>0.8361163139343262</v>
+        <v>0.6357388496398926</v>
       </c>
     </row>
     <row r="45">
@@ -1244,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.229909673333168</v>
+        <v>0.4414702951908112</v>
       </c>
     </row>
     <row r="46">
@@ -1262,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>0.8878927826881409</v>
+        <v>0.8643794059753418</v>
       </c>
     </row>
     <row r="47">
@@ -1280,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.7890173196792603</v>
+        <v>0.7324144244194031</v>
       </c>
     </row>
     <row r="48">
@@ -1298,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="D48" t="n">
-        <v>0.766759991645813</v>
+        <v>0.7587654590606689</v>
       </c>
     </row>
     <row r="49">
@@ -1313,10 +1313,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.5097872614860535</v>
+        <v>0.3502878844738007</v>
       </c>
     </row>
     <row r="50">
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>0.4527827501296997</v>
+        <v>0.4270217418670654</v>
       </c>
     </row>
     <row r="51">
@@ -1352,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5620206594467163</v>
+        <v>0.7436496019363403</v>
       </c>
     </row>
     <row r="52">
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0507841445505619</v>
+        <v>0.08126440644264221</v>
       </c>
     </row>
     <row r="53">
@@ -1385,10 +1385,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0.5920760631561279</v>
+        <v>0.2828573286533356</v>
       </c>
     </row>
     <row r="54">
@@ -1406,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>0.7917254567146301</v>
+        <v>0.8288872241973877</v>
       </c>
     </row>
     <row r="55">
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.4279964566230774</v>
+        <v>0.3590312004089355</v>
       </c>
     </row>
     <row r="56">
@@ -1439,10 +1439,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>0.4749461114406586</v>
+        <v>0.6459195613861084</v>
       </c>
     </row>
     <row r="57">
@@ -1460,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1445198357105255</v>
+        <v>0.2269430160522461</v>
       </c>
     </row>
     <row r="58">
@@ -1478,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="D58" t="n">
-        <v>0.82768315076828</v>
+        <v>0.8229509592056274</v>
       </c>
     </row>
     <row r="59">
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="D59" t="n">
-        <v>0.6732674837112427</v>
+        <v>0.7895099520683289</v>
       </c>
     </row>
     <row r="60">
@@ -1514,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>0.9076248407363892</v>
+        <v>0.8976601958274841</v>
       </c>
     </row>
     <row r="61">
@@ -1532,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>0.8603790998458862</v>
+        <v>0.6911138892173767</v>
       </c>
     </row>
     <row r="62">
@@ -1550,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>0.6268876791000366</v>
+        <v>0.7324249148368835</v>
       </c>
     </row>
     <row r="63">
@@ -1568,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="D63" t="n">
-        <v>0.69300377368927</v>
+        <v>0.5695649385452271</v>
       </c>
     </row>
     <row r="64">
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4051770865917206</v>
+        <v>0.3720881342887878</v>
       </c>
     </row>
     <row r="65">
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>0.07653657346963882</v>
+        <v>0.09626663476228714</v>
       </c>
     </row>
     <row r="66">
@@ -1622,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>0.5595602989196777</v>
+        <v>0.746989369392395</v>
       </c>
     </row>
     <row r="67">
@@ -1637,10 +1637,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>0.6175572872161865</v>
+        <v>0.1907045394182205</v>
       </c>
     </row>
     <row r="68">
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="D68" t="n">
-        <v>0.5890623331069946</v>
+        <v>0.590224027633667</v>
       </c>
     </row>
     <row r="69">
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6742767095565796</v>
+        <v>0.6740698218345642</v>
       </c>
     </row>
     <row r="70">
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2918533682823181</v>
+        <v>0.21464604139328</v>
       </c>
     </row>
     <row r="71">
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>0.1933367252349854</v>
+        <v>0.2641399502754211</v>
       </c>
     </row>
     <row r="72">
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.3219210803508759</v>
+        <v>0.277616560459137</v>
       </c>
     </row>
     <row r="73">
@@ -1748,7 +1748,7 @@
         <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>0.8520599603652954</v>
+        <v>0.8923956155776978</v>
       </c>
     </row>
     <row r="74">
@@ -1763,10 +1763,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>0.2982775568962097</v>
+        <v>0.6170204281806946</v>
       </c>
     </row>
     <row r="75">
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.06310324370861053</v>
+        <v>0.1127720177173615</v>
       </c>
     </row>
     <row r="76">
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>0.1428236216306686</v>
+        <v>0.4118671715259552</v>
       </c>
     </row>
     <row r="77">
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="D77" t="n">
-        <v>0.6283961534500122</v>
+        <v>0.6918544769287109</v>
       </c>
     </row>
     <row r="78">
@@ -1838,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="D78" t="n">
-        <v>0.7583253979682922</v>
+        <v>0.8272613286972046</v>
       </c>
     </row>
     <row r="79">
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>0.1540525108575821</v>
+        <v>0.1887997835874557</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New best performing classical pca model
</commit_message>
<xml_diff>
--- a/predictions/classical_pca_predictions.xlsx
+++ b/predictions/classical_pca_predictions.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,392 +463,392 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Green Bay Packers</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5876173973083496</v>
+        <v>0.6786988973617554</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5127014517784119</v>
+        <v>0.4432582855224609</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8669266700744629</v>
+        <v>0.2975495457649231</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8246411681175232</v>
+        <v>0.1903766244649887</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.06286820024251938</v>
+        <v>0.4933071434497833</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8776209354400635</v>
+        <v>0.6472492218017578</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7707201838493347</v>
+        <v>0.5157468318939209</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3048694133758545</v>
+        <v>0.6766335368156433</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.495371550321579</v>
+        <v>0.7066811323165894</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2303283959627151</v>
+        <v>0.1451976448297501</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Green Bay Packers</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1857190877199173</v>
+        <v>0.809389591217041</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8674956560134888</v>
+        <v>0.2298402935266495</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8751955032348633</v>
+        <v>0.5444283485412598</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4216914474964142</v>
+        <v>0.5707367658615112</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2624797523021698</v>
+        <v>0.6635158061981201</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>New York Giants</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7577654123306274</v>
+        <v>0.7384364604949951</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="C18" t="n">
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6054984331130981</v>
+        <v>0.92219477891922</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4093546569347382</v>
+        <v>0.6207009553909302</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3960031867027283</v>
+        <v>0.4275381565093994</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>New England Patriots</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1320594996213913</v>
+        <v>0.5824572443962097</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>New York Giants</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6615296602249146</v>
+        <v>0.7477089166641235</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="C23" t="n">
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7411167621612549</v>
+        <v>0.9320067763328552</v>
       </c>
     </row>
     <row r="24">
@@ -859,20 +859,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4433744549751282</v>
+        <v>0.8191788196563721</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>San Francisco 49ers</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -884,175 +884,175 @@
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7918363809585571</v>
+        <v>0.8950821161270142</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9470779895782471</v>
+        <v>0.48153156042099</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>0.04427319392561913</v>
+        <v>0.5472047328948975</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Denver Broncos</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>Green Bay Packers</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Chicago Bears</t>
-        </is>
-      </c>
       <c r="C28" t="n">
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>0.8608905076980591</v>
+        <v>0.6477506160736084</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Carolina Panthers</t>
         </is>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3152673542499542</v>
+        <v>0.3413574397563934</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="C30" t="n">
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7652621269226074</v>
+        <v>0.8667417168617249</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5419816970825195</v>
+        <v>0.4747653603553772</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="C32" t="n">
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>0.7014244794845581</v>
+        <v>0.5281369090080261</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>Green Bay Packers</t>
         </is>
       </c>
       <c r="C33" t="n">
         <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>0.722465991973877</v>
+        <v>0.5732511281967163</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0.907707154750824</v>
+        <v>0.3249567449092865</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1064,43 +1064,43 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6762729287147522</v>
+        <v>0.5952136516571045</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1494694650173187</v>
+        <v>0.1134684458374977</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0.453951358795166</v>
+        <v>0.681637167930603</v>
       </c>
     </row>
     <row r="38">
@@ -1111,590 +1111,590 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8986181616783142</v>
+        <v>0.822587251663208</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Carolina Panthers</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="C39" t="n">
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>0.9582871198654175</v>
+        <v>0.5124905109405518</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8870537877082825</v>
+        <v>0.3997949659824371</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="C41" t="n">
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9650564789772034</v>
+        <v>0.7029480338096619</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="C42" t="n">
         <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>0.5881452560424805</v>
+        <v>0.5902425646781921</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="C43" t="n">
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>0.7852417826652527</v>
+        <v>0.6897406578063965</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Green Bay Packers</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="C44" t="n">
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>0.6357388496398926</v>
+        <v>0.8299673199653625</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>0.4414702951908112</v>
+        <v>0.7259016036987305</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>New England Patriots</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.8643794059753418</v>
+        <v>0.1240127682685852</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>San Francisco 49ers</t>
         </is>
       </c>
       <c r="C47" t="n">
         <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.7324144244194031</v>
+        <v>0.6072885990142822</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.7587654590606689</v>
+        <v>0.4899943470954895</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Green Bay Packers</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.3502878844738007</v>
+        <v>0.1459715217351913</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>0.4270217418670654</v>
+        <v>0.4122688770294189</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>New York Giants</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>0.7436496019363403</v>
+        <v>0.2189405709505081</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>0.08126440644264221</v>
+        <v>0.5734624266624451</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Green Bay Packers</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>0.2828573286533356</v>
+        <v>0.7846308946609497</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>New York Giants</t>
+          <t>Carolina Panthers</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.8288872241973877</v>
+        <v>0.2131585031747818</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.3590312004089355</v>
+        <v>0.4153362214565277</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>0.6459195613861084</v>
+        <v>0.4510194361209869</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2269430160522461</v>
+        <v>0.6782031059265137</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="C58" t="n">
         <v>1</v>
       </c>
       <c r="D58" t="n">
-        <v>0.8229509592056274</v>
+        <v>0.5777691602706909</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>New England Patriots</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.7895099520683289</v>
+        <v>0.04197001084685326</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0.8976601958274841</v>
+        <v>0.4902610778808594</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="C61" t="n">
         <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>0.6911138892173767</v>
+        <v>0.6395214796066284</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>San Francisco 49ers</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="C62" t="n">
         <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>0.7324249148368835</v>
+        <v>0.7033206820487976</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>0.5695649385452271</v>
+        <v>0.1631911098957062</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>0.3720881342887878</v>
+        <v>0.1004190593957901</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" t="n">
-        <v>0.09626663476228714</v>
+        <v>0.8841681480407715</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>San Francisco 49ers</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="C66" t="n">
         <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>0.746989369392395</v>
+        <v>0.5363420248031616</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>New York Giants</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>0.1907045394182205</v>
+        <v>0.8414907455444336</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>0.590224027633667</v>
+        <v>0.4962874948978424</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>Minnesota Vikings</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>Green Bay Packers</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Baltimore Ravens</t>
-        </is>
-      </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6740698218345642</v>
+        <v>0.1148182451725006</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="n">
-        <v>0.21464604139328</v>
+        <v>0.5915384292602539</v>
       </c>
     </row>
     <row r="71">
@@ -1705,20 +1705,20 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2641399502754211</v>
+        <v>0.6590469479560852</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1727,136 +1727,136 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72" t="n">
-        <v>0.277616560459137</v>
+        <v>0.5290435552597046</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="C73" t="n">
         <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>0.8923956155776978</v>
+        <v>0.7793537378311157</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>New England Patriots</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>Miami Dolphins</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Tampa Bay Buccaneers</t>
-        </is>
-      </c>
       <c r="C74" t="n">
         <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>0.6170204281806946</v>
+        <v>0.7696195244789124</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>New York Giants</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="C75" t="n">
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.1127720177173615</v>
+        <v>0.4456982612609863</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" t="n">
-        <v>0.4118671715259552</v>
+        <v>0.8558508157730103</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>0.6918544769287109</v>
+        <v>0.3682286739349365</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Carolina Panthers</t>
         </is>
       </c>
       <c r="C78" t="n">
         <v>1</v>
       </c>
       <c r="D78" t="n">
-        <v>0.8272613286972046</v>
+        <v>0.5203900337219238</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79" t="n">
-        <v>0.1887997835874557</v>
+        <v>0.9304859638214111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project Models and stats done
</commit_message>
<xml_diff>
--- a/predictions/classical_pca_predictions.xlsx
+++ b/predictions/classical_pca_predictions.xlsx
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5422162413597107</v>
+        <v>0.4598758518695831</v>
       </c>
     </row>
     <row r="3">
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3413213491439819</v>
+        <v>0.28061443567276</v>
       </c>
     </row>
     <row r="4">
@@ -503,10 +503,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5243908762931824</v>
+        <v>0.4257664084434509</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3016238808631897</v>
+        <v>0.4928802251815796</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2101276814937592</v>
+        <v>0.2253124266862869</v>
       </c>
     </row>
     <row r="7">
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5723477602005005</v>
+        <v>0.4928478896617889</v>
       </c>
     </row>
     <row r="8">
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6444730758666992</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="9">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3565127849578857</v>
+        <v>0.4815551042556763</v>
       </c>
     </row>
     <row r="10">
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2652007043361664</v>
+        <v>0.2523618638515472</v>
       </c>
     </row>
     <row r="11">
@@ -629,10 +629,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6293562650680542</v>
+        <v>0.4697722196578979</v>
       </c>
     </row>
     <row r="12">
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5684676170349121</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="13">
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2026762068271637</v>
+        <v>0.3603732287883759</v>
       </c>
     </row>
     <row r="14">
@@ -686,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9557652473449707</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="15">
@@ -701,10 +701,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4573135375976562</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="16">
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3547945022583008</v>
+        <v>0.3452500998973846</v>
       </c>
     </row>
     <row r="17">
@@ -737,10 +737,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4442624151706696</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="18">
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.481218159198761</v>
+        <v>0.3106700479984283</v>
       </c>
     </row>
     <row r="19">
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.219781681895256</v>
+        <v>0.2074257433414459</v>
       </c>
     </row>
     <row r="20">
@@ -794,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3092500269412994</v>
+        <v>0.3105953931808472</v>
       </c>
     </row>
     <row r="21">
@@ -812,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3035755157470703</v>
+        <v>0.3164584934711456</v>
       </c>
     </row>
     <row r="22">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5151457786560059</v>
+        <v>0.4747440218925476</v>
       </c>
     </row>
     <row r="23">
@@ -848,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1336632072925568</v>
+        <v>0.3409002721309662</v>
       </c>
     </row>
     <row r="24">
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5479538440704346</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="25">
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2866270244121552</v>
+        <v>0.4446874260902405</v>
       </c>
     </row>
     <row r="26">
@@ -899,10 +899,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4841506779193878</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="27">
@@ -920,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2388443201780319</v>
+        <v>0.4245058596134186</v>
       </c>
     </row>
     <row r="28">
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0.08913628756999969</v>
+        <v>0.1968528181314468</v>
       </c>
     </row>
     <row r="29">
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3140361607074738</v>
+        <v>0.4138520359992981</v>
       </c>
     </row>
     <row r="30">
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0.3229212462902069</v>
+        <v>0.4233212769031525</v>
       </c>
     </row>
     <row r="31">
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4570416510105133</v>
+        <v>0.4211584627628326</v>
       </c>
     </row>
     <row r="32">
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5306990742683411</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="33">
@@ -1028,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.255555272102356</v>
+        <v>0.2359626442193985</v>
       </c>
     </row>
     <row r="34">
@@ -1046,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1674075126647949</v>
+        <v>0.2342540472745895</v>
       </c>
     </row>
     <row r="35">
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8235510587692261</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="36">
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.2598710358142853</v>
+        <v>0.391911655664444</v>
       </c>
     </row>
     <row r="37">
@@ -1097,10 +1097,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0.7105162739753723</v>
+        <v>0.494405210018158</v>
       </c>
     </row>
     <row r="38">
@@ -1115,10 +1115,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8385072350502014</v>
+        <v>0.4463329613208771</v>
       </c>
     </row>
     <row r="39">
@@ -1136,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.1172383427619934</v>
+        <v>0.392715722322464</v>
       </c>
     </row>
     <row r="40">
@@ -1151,10 +1151,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8059231042861938</v>
+        <v>0.2559272050857544</v>
       </c>
     </row>
     <row r="41">
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5800024271011353</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="42">
@@ -1190,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>0.6584905385971069</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="43">
@@ -1208,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>0.8189316391944885</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="44">
@@ -1226,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>0.5996783971786499</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="45">
@@ -1244,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.435863196849823</v>
+        <v>0.3382506966590881</v>
       </c>
     </row>
     <row r="46">
@@ -1262,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>0.7564249038696289</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
     <row r="47">
@@ -1280,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0.479569137096405</v>
+        <v>0.4303871393203735</v>
       </c>
     </row>
     <row r="48">
@@ -1295,10 +1295,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.6223937273025513</v>
+        <v>0.4572837054729462</v>
       </c>
     </row>
     <row r="49">
@@ -1316,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>0.9666643142700195</v>
+        <v>0.504837691783905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>